<commit_message>
added android and ios
</commit_message>
<xml_diff>
--- a/UITesting.xlsx
+++ b/UITesting.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\nodeApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3490F4DF-365A-4379-9A87-760645363E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CB46C1-9F7E-44B9-A3C4-5CF36FAAB97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33060" yWindow="-3180" windowWidth="19305" windowHeight="10545" xr2:uid="{9A7F5B4D-2907-4E98-9930-CE5F8021C7E0}"/>
+    <workbookView xWindow="-38505" yWindow="-1800" windowWidth="38400" windowHeight="10545" xr2:uid="{9A7F5B4D-2907-4E98-9930-CE5F8021C7E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Questions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>username</t>
   </si>
@@ -93,6 +94,46 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>UI should display a message saying the user account is successfully created.</t>
+  </si>
+  <si>
+    <t>listname1001</t>
+  </si>
+  <si>
+    <t>item11001</t>
+  </si>
+  <si>
+    <t>quantity1</t>
+  </si>
+  <si>
+    <t>quantity2</t>
+  </si>
+  <si>
+    <t>quantity3</t>
+  </si>
+  <si>
+    <t>item21001</t>
+  </si>
+  <si>
+    <t>item31001</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>How to make the app available in all the regions of the world?</t>
+  </si>
+  <si>
+    <t>Quantity should be defaulted to 1. 
+Quantity should be increased or decreased with + and - buttons</t>
   </si>
 </sst>
 </file>
@@ -143,9 +184,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -481,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDCA8DB4-A2F8-486D-A8DD-55184F7F4D96}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -494,12 +538,15 @@
     <col min="3" max="3" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.6328125" customWidth="1"/>
+    <col min="6" max="6" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="9.453125" customWidth="1"/>
+    <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="66.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -516,24 +563,33 @@
         <v>9</v>
       </c>
       <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -549,8 +605,14 @@
       <c r="E4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2</v>
       </c>
@@ -560,23 +622,50 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -593,4 +682,38 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF00C2D5-802A-4C2C-8582-0685F003B40E}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="53.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>